<commit_message>
Making inputs allow for leading 0
</commit_message>
<xml_diff>
--- a/pyexcel.xlsx
+++ b/pyexcel.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Grocery Rescue" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Grocery Rescue" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
@@ -1007,7 +1007,7 @@
     <row r="6" ht="15.75" customHeight="1" s="39">
       <c r="A6" s="58" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>1608894</t>
         </is>
       </c>
       <c r="B6" s="59" t="n"/>
@@ -1024,19 +1024,19 @@
         <v/>
       </c>
       <c r="F6" s="62" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G6" s="62" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H6" s="62" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I6" s="62" t="n">
-        <v>54</v>
+        <v>150</v>
       </c>
       <c r="J6" s="62" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="K6" s="62" t="n"/>
       <c r="L6" s="62" t="n"/>
@@ -1052,7 +1052,7 @@
     <row r="7" ht="15.75" customHeight="1" s="39">
       <c r="A7" s="58" t="inlineStr">
         <is>
-          <t>1234</t>
+          <t>106241</t>
         </is>
       </c>
       <c r="B7" s="59" t="n"/>
@@ -1067,19 +1067,19 @@
         <v/>
       </c>
       <c r="F7" s="62" t="n">
-        <v>7897987978989</v>
+        <v>60</v>
       </c>
       <c r="G7" s="62" t="n">
-        <v>4</v>
+        <v>105</v>
       </c>
       <c r="H7" s="62" t="n">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="I7" s="62" t="n">
-        <v>4</v>
+        <v>220</v>
       </c>
       <c r="J7" s="62" t="n">
-        <v>4</v>
+        <v>75</v>
       </c>
       <c r="K7" s="62" t="n"/>
       <c r="L7" s="62" t="n"/>
@@ -1095,7 +1095,7 @@
     <row r="8" ht="15.75" customHeight="1" s="39">
       <c r="A8" s="63" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1608883</t>
         </is>
       </c>
       <c r="B8" s="64" t="n"/>
@@ -1110,19 +1110,19 @@
         <v/>
       </c>
       <c r="F8" s="65" t="n">
-        <v>1</v>
+        <v>245</v>
       </c>
       <c r="G8" s="65" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="H8" s="65" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I8" s="65" t="n">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="J8" s="65" t="n">
-        <v>1</v>
+        <v>155</v>
       </c>
       <c r="K8" s="62" t="n"/>
       <c r="L8" s="62" t="n"/>
@@ -1136,19 +1136,37 @@
       <c r="T8" s="62" t="n"/>
     </row>
     <row r="9" ht="15.75" customHeight="1" s="39">
-      <c r="A9" s="63" t="n"/>
+      <c r="A9" s="63" t="inlineStr">
+        <is>
+          <t>63366</t>
+        </is>
+      </c>
       <c r="B9" s="64" t="n"/>
       <c r="C9" s="60" t="n"/>
-      <c r="D9" s="60" t="n"/>
+      <c r="D9" s="60" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
       <c r="E9" s="61">
         <f>SUM(F9:T9)</f>
         <v/>
       </c>
-      <c r="F9" s="65" t="n"/>
-      <c r="G9" s="65" t="n"/>
-      <c r="H9" s="65" t="n"/>
-      <c r="I9" s="65" t="n"/>
-      <c r="J9" s="65" t="n"/>
+      <c r="F9" s="65" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="65" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="65" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="65" t="n">
+        <v>465</v>
+      </c>
+      <c r="J9" s="65" t="n">
+        <v>0</v>
+      </c>
       <c r="K9" s="62" t="n"/>
       <c r="L9" s="62" t="n"/>
       <c r="M9" s="62" t="n"/>
@@ -1161,19 +1179,37 @@
       <c r="T9" s="62" t="n"/>
     </row>
     <row r="10" ht="15.75" customHeight="1" s="39">
-      <c r="A10" s="63" t="n"/>
+      <c r="A10" s="63" t="inlineStr">
+        <is>
+          <t>10201</t>
+        </is>
+      </c>
       <c r="B10" s="64" t="n"/>
       <c r="C10" s="60" t="n"/>
-      <c r="D10" s="60" t="n"/>
+      <c r="D10" s="60" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
       <c r="E10" s="61">
         <f>SUM(F10:T10)</f>
         <v/>
       </c>
-      <c r="F10" s="65" t="n"/>
-      <c r="G10" s="65" t="n"/>
-      <c r="H10" s="65" t="n"/>
-      <c r="I10" s="65" t="n"/>
-      <c r="J10" s="65" t="n"/>
+      <c r="F10" s="65" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="65" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="65" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="65" t="n">
+        <v>485</v>
+      </c>
+      <c r="J10" s="65" t="n">
+        <v>100</v>
+      </c>
       <c r="K10" s="62" t="n"/>
       <c r="L10" s="62" t="n"/>
       <c r="M10" s="62" t="n"/>
@@ -1186,19 +1222,37 @@
       <c r="T10" s="62" t="n"/>
     </row>
     <row r="11" ht="15.75" customHeight="1" s="39">
-      <c r="A11" s="58" t="n"/>
+      <c r="A11" s="58" t="inlineStr">
+        <is>
+          <t>101418</t>
+        </is>
+      </c>
       <c r="B11" s="59" t="n"/>
       <c r="C11" s="60" t="n"/>
-      <c r="D11" s="60" t="n"/>
+      <c r="D11" s="60" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
       <c r="E11" s="61">
         <f>SUM(F11:T11)</f>
         <v/>
       </c>
-      <c r="F11" s="62" t="n"/>
-      <c r="G11" s="62" t="n"/>
-      <c r="H11" s="62" t="n"/>
-      <c r="I11" s="62" t="n"/>
-      <c r="J11" s="62" t="n"/>
+      <c r="F11" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="62" t="n">
+        <v>90</v>
+      </c>
+      <c r="H11" s="62" t="n">
+        <v>150</v>
+      </c>
+      <c r="I11" s="62" t="n">
+        <v>365</v>
+      </c>
+      <c r="J11" s="62" t="n">
+        <v>0</v>
+      </c>
       <c r="K11" s="62" t="n"/>
       <c r="L11" s="62" t="n"/>
       <c r="M11" s="62" t="n"/>
@@ -1211,19 +1265,37 @@
       <c r="T11" s="62" t="n"/>
     </row>
     <row r="12" ht="15.75" customHeight="1" s="39">
-      <c r="A12" s="58" t="n"/>
+      <c r="A12" s="58" t="inlineStr">
+        <is>
+          <t>15025</t>
+        </is>
+      </c>
       <c r="B12" s="59" t="n"/>
       <c r="C12" s="60" t="n"/>
-      <c r="D12" s="60" t="n"/>
+      <c r="D12" s="60" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
       <c r="E12" s="61">
         <f>SUM(F12:T12)</f>
         <v/>
       </c>
-      <c r="F12" s="62" t="n"/>
-      <c r="G12" s="62" t="n"/>
-      <c r="H12" s="62" t="n"/>
-      <c r="I12" s="62" t="n"/>
-      <c r="J12" s="62" t="n"/>
+      <c r="F12" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="62" t="n">
+        <v>110</v>
+      </c>
+      <c r="H12" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="62" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J12" s="62" t="n">
+        <v>0</v>
+      </c>
       <c r="K12" s="62" t="n"/>
       <c r="L12" s="62" t="n"/>
       <c r="M12" s="62" t="n"/>
@@ -1236,19 +1308,37 @@
       <c r="T12" s="62" t="n"/>
     </row>
     <row r="13" ht="15.75" customHeight="1" s="39">
-      <c r="A13" s="58" t="n"/>
+      <c r="A13" s="58" t="inlineStr">
+        <is>
+          <t>47012</t>
+        </is>
+      </c>
       <c r="B13" s="59" t="n"/>
       <c r="C13" s="60" t="n"/>
-      <c r="D13" s="60" t="n"/>
+      <c r="D13" s="60" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
       <c r="E13" s="61">
         <f>SUM(F13:T13)</f>
         <v/>
       </c>
-      <c r="F13" s="62" t="n"/>
-      <c r="G13" s="62" t="n"/>
-      <c r="H13" s="62" t="n"/>
-      <c r="I13" s="62" t="n"/>
-      <c r="J13" s="62" t="n"/>
+      <c r="F13" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="62" t="n">
+        <v>450</v>
+      </c>
+      <c r="J13" s="62" t="n">
+        <v>0</v>
+      </c>
       <c r="K13" s="62" t="n"/>
       <c r="L13" s="62" t="n"/>
       <c r="M13" s="62" t="n"/>
@@ -1261,19 +1351,37 @@
       <c r="T13" s="62" t="n"/>
     </row>
     <row r="14" ht="15.75" customHeight="1" s="39">
-      <c r="A14" s="63" t="n"/>
+      <c r="A14" s="63" t="inlineStr">
+        <is>
+          <t>15025</t>
+        </is>
+      </c>
       <c r="B14" s="64" t="n"/>
       <c r="C14" s="60" t="n"/>
-      <c r="D14" s="60" t="n"/>
+      <c r="D14" s="60" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
       <c r="E14" s="61">
         <f>SUM(F14:T14)</f>
         <v/>
       </c>
-      <c r="F14" s="65" t="n"/>
-      <c r="G14" s="65" t="n"/>
-      <c r="H14" s="65" t="n"/>
-      <c r="I14" s="65" t="n"/>
-      <c r="J14" s="65" t="n"/>
+      <c r="F14" s="65" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="65" t="n">
+        <v>110</v>
+      </c>
+      <c r="H14" s="65" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="65" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J14" s="65" t="n">
+        <v>0</v>
+      </c>
       <c r="K14" s="62" t="n"/>
       <c r="L14" s="62" t="n"/>
       <c r="M14" s="62" t="n"/>
@@ -1286,19 +1394,37 @@
       <c r="T14" s="62" t="n"/>
     </row>
     <row r="15" ht="15.75" customHeight="1" s="39">
-      <c r="A15" s="58" t="n"/>
+      <c r="A15" s="58" t="inlineStr">
+        <is>
+          <t>47012</t>
+        </is>
+      </c>
       <c r="B15" s="59" t="n"/>
       <c r="C15" s="60" t="n"/>
-      <c r="D15" s="60" t="n"/>
+      <c r="D15" s="60" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
       <c r="E15" s="61">
         <f>SUM(F15:T15)</f>
         <v/>
       </c>
-      <c r="F15" s="62" t="n"/>
-      <c r="G15" s="62" t="n"/>
-      <c r="H15" s="62" t="n"/>
-      <c r="I15" s="62" t="n"/>
-      <c r="J15" s="62" t="n"/>
+      <c r="F15" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="62" t="n">
+        <v>450</v>
+      </c>
+      <c r="J15" s="62" t="n">
+        <v>0</v>
+      </c>
       <c r="K15" s="62" t="n"/>
       <c r="L15" s="62" t="n"/>
       <c r="M15" s="62" t="n"/>
@@ -1311,19 +1437,37 @@
       <c r="T15" s="62" t="n"/>
     </row>
     <row r="16" ht="15.75" customHeight="1" s="39">
-      <c r="A16" s="58" t="n"/>
+      <c r="A16" s="58" t="inlineStr">
+        <is>
+          <t>34000</t>
+        </is>
+      </c>
       <c r="B16" s="59" t="n"/>
       <c r="C16" s="60" t="n"/>
-      <c r="D16" s="60" t="n"/>
+      <c r="D16" s="60" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
       <c r="E16" s="61">
         <f>SUM(F16:T16)</f>
         <v/>
       </c>
-      <c r="F16" s="62" t="n"/>
-      <c r="G16" s="62" t="n"/>
-      <c r="H16" s="62" t="n"/>
-      <c r="I16" s="62" t="n"/>
-      <c r="J16" s="62" t="n"/>
+      <c r="F16" s="62" t="n">
+        <v>285</v>
+      </c>
+      <c r="G16" s="62" t="n">
+        <v>110</v>
+      </c>
+      <c r="H16" s="62" t="n">
+        <v>30</v>
+      </c>
+      <c r="I16" s="62" t="n">
+        <v>510</v>
+      </c>
+      <c r="J16" s="62" t="n">
+        <v>0</v>
+      </c>
       <c r="K16" s="62" t="n"/>
       <c r="L16" s="62" t="n"/>
       <c r="M16" s="62" t="n"/>
@@ -1336,19 +1480,37 @@
       <c r="T16" s="62" t="n"/>
     </row>
     <row r="17" ht="15.75" customHeight="1" s="39">
-      <c r="A17" s="58" t="n"/>
+      <c r="A17" s="58" t="inlineStr">
+        <is>
+          <t>226547</t>
+        </is>
+      </c>
       <c r="B17" s="59" t="n"/>
       <c r="C17" s="60" t="n"/>
-      <c r="D17" s="60" t="n"/>
+      <c r="D17" s="60" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
       <c r="E17" s="61">
         <f>SUM(F17:T17)</f>
         <v/>
       </c>
-      <c r="F17" s="62" t="n"/>
-      <c r="G17" s="62" t="n"/>
-      <c r="H17" s="62" t="n"/>
-      <c r="I17" s="62" t="n"/>
-      <c r="J17" s="62" t="n"/>
+      <c r="F17" s="62" t="n">
+        <v>1100</v>
+      </c>
+      <c r="G17" s="62" t="n">
+        <v>130</v>
+      </c>
+      <c r="H17" s="62" t="n">
+        <v>700</v>
+      </c>
+      <c r="I17" s="62" t="n">
+        <v>1500</v>
+      </c>
+      <c r="J17" s="62" t="n">
+        <v>0</v>
+      </c>
       <c r="K17" s="62" t="n"/>
       <c r="L17" s="62" t="n"/>
       <c r="M17" s="62" t="n"/>
@@ -1361,19 +1523,37 @@
       <c r="T17" s="62" t="n"/>
     </row>
     <row r="18" ht="15.75" customHeight="1" s="39">
-      <c r="A18" s="58" t="n"/>
+      <c r="A18" s="58" t="inlineStr">
+        <is>
+          <t>1609005</t>
+        </is>
+      </c>
       <c r="B18" s="59" t="n"/>
       <c r="C18" s="60" t="n"/>
-      <c r="D18" s="60" t="n"/>
+      <c r="D18" s="60" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
       <c r="E18" s="61">
         <f>SUM(F18:T18)</f>
         <v/>
       </c>
-      <c r="F18" s="62" t="n"/>
-      <c r="G18" s="62" t="n"/>
-      <c r="H18" s="62" t="n"/>
-      <c r="I18" s="62" t="n"/>
-      <c r="J18" s="62" t="n"/>
+      <c r="F18" s="62" t="n">
+        <v>500</v>
+      </c>
+      <c r="G18" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="62" t="n">
+        <v>400</v>
+      </c>
+      <c r="J18" s="62" t="n">
+        <v>0</v>
+      </c>
       <c r="K18" s="62" t="n"/>
       <c r="L18" s="62" t="n"/>
       <c r="M18" s="62" t="n"/>
@@ -1386,19 +1566,37 @@
       <c r="T18" s="62" t="n"/>
     </row>
     <row r="19" ht="15.75" customHeight="1" s="39">
-      <c r="A19" s="58" t="n"/>
+      <c r="A19" s="58" t="inlineStr">
+        <is>
+          <t>1001188</t>
+        </is>
+      </c>
       <c r="B19" s="59" t="n"/>
       <c r="C19" s="60" t="n"/>
-      <c r="D19" s="60" t="n"/>
+      <c r="D19" s="60" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
       <c r="E19" s="61">
         <f>SUM(F19:T19)</f>
         <v/>
       </c>
-      <c r="F19" s="62" t="n"/>
-      <c r="G19" s="62" t="n"/>
-      <c r="H19" s="62" t="n"/>
-      <c r="I19" s="62" t="n"/>
-      <c r="J19" s="62" t="n"/>
+      <c r="F19" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="62" t="n">
+        <v>285</v>
+      </c>
+      <c r="J19" s="62" t="n">
+        <v>0</v>
+      </c>
       <c r="K19" s="62" t="n"/>
       <c r="L19" s="62" t="n"/>
       <c r="M19" s="62" t="n"/>
@@ -1411,19 +1609,37 @@
       <c r="T19" s="62" t="n"/>
     </row>
     <row r="20" ht="15.75" customHeight="1" s="39">
-      <c r="A20" s="58" t="n"/>
+      <c r="A20" s="58" t="inlineStr">
+        <is>
+          <t>1001265</t>
+        </is>
+      </c>
       <c r="B20" s="59" t="n"/>
       <c r="C20" s="60" t="n"/>
-      <c r="D20" s="60" t="n"/>
+      <c r="D20" s="60" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
       <c r="E20" s="61">
         <f>SUM(F20:T20)</f>
         <v/>
       </c>
-      <c r="F20" s="62" t="n"/>
-      <c r="G20" s="62" t="n"/>
-      <c r="H20" s="62" t="n"/>
-      <c r="I20" s="62" t="n"/>
-      <c r="J20" s="62" t="n"/>
+      <c r="F20" s="62" t="n">
+        <v>80</v>
+      </c>
+      <c r="G20" s="62" t="n">
+        <v>150</v>
+      </c>
+      <c r="H20" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="62" t="n">
+        <v>290</v>
+      </c>
+      <c r="J20" s="62" t="n">
+        <v>0</v>
+      </c>
       <c r="K20" s="62" t="n"/>
       <c r="L20" s="62" t="n"/>
       <c r="M20" s="62" t="n"/>
@@ -1436,19 +1652,37 @@
       <c r="T20" s="62" t="n"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" s="39">
-      <c r="A21" s="58" t="n"/>
+      <c r="A21" s="58" t="inlineStr">
+        <is>
+          <t>291066</t>
+        </is>
+      </c>
       <c r="B21" s="59" t="n"/>
       <c r="C21" s="60" t="n"/>
-      <c r="D21" s="60" t="n"/>
+      <c r="D21" s="60" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
       <c r="E21" s="61">
         <f>SUM(F21:T21)</f>
         <v/>
       </c>
-      <c r="F21" s="62" t="n"/>
-      <c r="G21" s="62" t="n"/>
-      <c r="H21" s="62" t="n"/>
-      <c r="I21" s="62" t="n"/>
-      <c r="J21" s="62" t="n"/>
+      <c r="F21" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="62" t="n">
+        <v>20</v>
+      </c>
+      <c r="J21" s="62" t="n">
+        <v>305</v>
+      </c>
       <c r="K21" s="62" t="n"/>
       <c r="L21" s="62" t="n"/>
       <c r="M21" s="62" t="n"/>
@@ -1461,19 +1695,37 @@
       <c r="T21" s="62" t="n"/>
     </row>
     <row r="22" ht="15.75" customHeight="1" s="39">
-      <c r="A22" s="58" t="n"/>
+      <c r="A22" s="58" t="inlineStr">
+        <is>
+          <t>100234</t>
+        </is>
+      </c>
       <c r="B22" s="59" t="n"/>
       <c r="C22" s="60" t="n"/>
-      <c r="D22" s="60" t="n"/>
+      <c r="D22" s="60" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
       <c r="E22" s="61">
         <f>SUM(F22:T22)</f>
         <v/>
       </c>
-      <c r="F22" s="62" t="n"/>
-      <c r="G22" s="62" t="n"/>
-      <c r="H22" s="62" t="n"/>
-      <c r="I22" s="62" t="n"/>
-      <c r="J22" s="62" t="n"/>
+      <c r="F22" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" s="62" t="n">
+        <v>855</v>
+      </c>
+      <c r="J22" s="62" t="n">
+        <v>35</v>
+      </c>
       <c r="K22" s="62" t="n"/>
       <c r="L22" s="62" t="n"/>
       <c r="M22" s="62" t="n"/>
@@ -1486,19 +1738,37 @@
       <c r="T22" s="62" t="n"/>
     </row>
     <row r="23" ht="15.75" customHeight="1" s="39">
-      <c r="A23" s="58" t="n"/>
+      <c r="A23" s="58" t="inlineStr">
+        <is>
+          <t>1608719</t>
+        </is>
+      </c>
       <c r="B23" s="59" t="n"/>
       <c r="C23" s="60" t="n"/>
-      <c r="D23" s="60" t="n"/>
+      <c r="D23" s="60" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
       <c r="E23" s="61">
         <f>SUM(F23:T23)</f>
         <v/>
       </c>
-      <c r="F23" s="65" t="n"/>
-      <c r="G23" s="65" t="n"/>
-      <c r="H23" s="65" t="n"/>
-      <c r="I23" s="65" t="n"/>
-      <c r="J23" s="65" t="n"/>
+      <c r="F23" s="65" t="n">
+        <v>205</v>
+      </c>
+      <c r="G23" s="65" t="n">
+        <v>135</v>
+      </c>
+      <c r="H23" s="65" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" s="65" t="n">
+        <v>195</v>
+      </c>
+      <c r="J23" s="65" t="n">
+        <v>515</v>
+      </c>
       <c r="K23" s="62" t="n"/>
       <c r="L23" s="62" t="n"/>
       <c r="M23" s="62" t="n"/>
@@ -1511,19 +1781,37 @@
       <c r="T23" s="62" t="n"/>
     </row>
     <row r="24" ht="15.75" customHeight="1" s="39">
-      <c r="A24" s="58" t="n"/>
+      <c r="A24" s="58" t="inlineStr">
+        <is>
+          <t>147832</t>
+        </is>
+      </c>
       <c r="B24" s="59" t="n"/>
       <c r="C24" s="60" t="n"/>
-      <c r="D24" s="60" t="n"/>
+      <c r="D24" s="60" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
       <c r="E24" s="61">
         <f>SUM(F24:T24)</f>
         <v/>
       </c>
-      <c r="F24" s="62" t="n"/>
-      <c r="G24" s="62" t="n"/>
-      <c r="H24" s="62" t="n"/>
-      <c r="I24" s="62" t="n"/>
-      <c r="J24" s="62" t="n"/>
+      <c r="F24" s="62" t="n">
+        <v>2735</v>
+      </c>
+      <c r="G24" s="62" t="n">
+        <v>225</v>
+      </c>
+      <c r="H24" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" s="62" t="n">
+        <v>2120</v>
+      </c>
+      <c r="J24" s="62" t="n">
+        <v>0</v>
+      </c>
       <c r="K24" s="62" t="n"/>
       <c r="L24" s="62" t="n"/>
       <c r="M24" s="62" t="n"/>
@@ -1536,19 +1824,37 @@
       <c r="T24" s="62" t="n"/>
     </row>
     <row r="25" ht="15.75" customHeight="1" s="39">
-      <c r="A25" s="58" t="n"/>
+      <c r="A25" s="58" t="inlineStr">
+        <is>
+          <t>1608526</t>
+        </is>
+      </c>
       <c r="B25" s="59" t="n"/>
       <c r="C25" s="60" t="n"/>
-      <c r="D25" s="60" t="n"/>
+      <c r="D25" s="60" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
       <c r="E25" s="61">
         <f>SUM(F25:T25)</f>
         <v/>
       </c>
-      <c r="F25" s="62" t="n"/>
-      <c r="G25" s="62" t="n"/>
-      <c r="H25" s="62" t="n"/>
-      <c r="I25" s="62" t="n"/>
-      <c r="J25" s="62" t="n"/>
+      <c r="F25" s="62" t="n">
+        <v>40</v>
+      </c>
+      <c r="G25" s="62" t="n">
+        <v>365</v>
+      </c>
+      <c r="H25" s="62" t="n">
+        <v>95</v>
+      </c>
+      <c r="I25" s="62" t="n">
+        <v>220</v>
+      </c>
+      <c r="J25" s="62" t="n">
+        <v>0</v>
+      </c>
       <c r="K25" s="62" t="n"/>
       <c r="L25" s="62" t="n"/>
       <c r="M25" s="62" t="n"/>
@@ -1561,19 +1867,37 @@
       <c r="T25" s="62" t="n"/>
     </row>
     <row r="26" ht="15.75" customHeight="1" s="39">
-      <c r="A26" s="58" t="n"/>
+      <c r="A26" s="58" t="inlineStr">
+        <is>
+          <t>1005313</t>
+        </is>
+      </c>
       <c r="B26" s="59" t="n"/>
       <c r="C26" s="60" t="n"/>
-      <c r="D26" s="60" t="n"/>
+      <c r="D26" s="60" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
       <c r="E26" s="61">
         <f>SUM(F26:T26)</f>
         <v/>
       </c>
-      <c r="F26" s="62" t="n"/>
-      <c r="G26" s="62" t="n"/>
-      <c r="H26" s="62" t="n"/>
-      <c r="I26" s="62" t="n"/>
-      <c r="J26" s="62" t="n"/>
+      <c r="F26" s="62" t="n">
+        <v>800</v>
+      </c>
+      <c r="G26" s="62" t="n">
+        <v>150</v>
+      </c>
+      <c r="H26" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="62" t="n">
+        <v>250</v>
+      </c>
+      <c r="J26" s="62" t="n">
+        <v>410</v>
+      </c>
       <c r="K26" s="62" t="n"/>
       <c r="L26" s="62" t="n"/>
       <c r="M26" s="62" t="n"/>
@@ -1586,19 +1910,37 @@
       <c r="T26" s="62" t="n"/>
     </row>
     <row r="27" ht="15.75" customHeight="1" s="39">
-      <c r="A27" s="58" t="n"/>
+      <c r="A27" s="58" t="inlineStr">
+        <is>
+          <t>102616</t>
+        </is>
+      </c>
       <c r="B27" s="59" t="n"/>
       <c r="C27" s="60" t="n"/>
-      <c r="D27" s="60" t="n"/>
+      <c r="D27" s="60" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
       <c r="E27" s="61">
         <f>SUM(F27:T27)</f>
         <v/>
       </c>
-      <c r="F27" s="62" t="n"/>
-      <c r="G27" s="62" t="n"/>
-      <c r="H27" s="62" t="n"/>
-      <c r="I27" s="62" t="n"/>
-      <c r="J27" s="62" t="n"/>
+      <c r="F27" s="62" t="n">
+        <v>200</v>
+      </c>
+      <c r="G27" s="62" t="n">
+        <v>75</v>
+      </c>
+      <c r="H27" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="62" t="n">
+        <v>150</v>
+      </c>
+      <c r="J27" s="62" t="n">
+        <v>0</v>
+      </c>
       <c r="K27" s="62" t="n"/>
       <c r="L27" s="62" t="n"/>
       <c r="M27" s="62" t="n"/>
@@ -1611,19 +1953,37 @@
       <c r="T27" s="62" t="n"/>
     </row>
     <row r="28" ht="15.75" customHeight="1" s="39">
-      <c r="A28" s="58" t="n"/>
+      <c r="A28" s="58" t="inlineStr">
+        <is>
+          <t>100243</t>
+        </is>
+      </c>
       <c r="B28" s="59" t="n"/>
       <c r="C28" s="60" t="n"/>
-      <c r="D28" s="60" t="n"/>
+      <c r="D28" s="60" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
       <c r="E28" s="61">
         <f>SUM(F28:T28)</f>
         <v/>
       </c>
-      <c r="F28" s="62" t="n"/>
-      <c r="G28" s="62" t="n"/>
-      <c r="H28" s="62" t="n"/>
-      <c r="I28" s="62" t="n"/>
-      <c r="J28" s="62" t="n"/>
+      <c r="F28" s="62" t="n">
+        <v>900</v>
+      </c>
+      <c r="G28" s="62" t="n">
+        <v>200</v>
+      </c>
+      <c r="H28" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="62" t="n">
+        <v>400</v>
+      </c>
+      <c r="J28" s="62" t="n">
+        <v>0</v>
+      </c>
       <c r="K28" s="62" t="n"/>
       <c r="L28" s="62" t="n"/>
       <c r="M28" s="62" t="n"/>
@@ -1636,19 +1996,37 @@
       <c r="T28" s="62" t="n"/>
     </row>
     <row r="29" ht="15.75" customHeight="1" s="39">
-      <c r="A29" s="58" t="n"/>
+      <c r="A29" s="58" t="inlineStr">
+        <is>
+          <t>23004</t>
+        </is>
+      </c>
       <c r="B29" s="59" t="n"/>
       <c r="C29" s="60" t="n"/>
-      <c r="D29" s="60" t="n"/>
+      <c r="D29" s="60" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
       <c r="E29" s="61">
         <f>SUM(F29:T29)</f>
         <v/>
       </c>
-      <c r="F29" s="62" t="n"/>
-      <c r="G29" s="62" t="n"/>
-      <c r="H29" s="62" t="n"/>
-      <c r="I29" s="62" t="n"/>
-      <c r="J29" s="62" t="n"/>
+      <c r="F29" s="62" t="n">
+        <v>75</v>
+      </c>
+      <c r="G29" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" s="62" t="n">
+        <v>0</v>
+      </c>
       <c r="K29" s="62" t="n"/>
       <c r="L29" s="62" t="n"/>
       <c r="M29" s="62" t="n"/>
@@ -1661,19 +2039,37 @@
       <c r="T29" s="62" t="n"/>
     </row>
     <row r="30" ht="15.75" customHeight="1" s="39">
-      <c r="A30" s="58" t="n"/>
+      <c r="A30" s="58" t="inlineStr">
+        <is>
+          <t>18383</t>
+        </is>
+      </c>
       <c r="B30" s="59" t="n"/>
       <c r="C30" s="60" t="n"/>
-      <c r="D30" s="60" t="n"/>
+      <c r="D30" s="60" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
       <c r="E30" s="61">
         <f>SUM(F30:T30)</f>
         <v/>
       </c>
-      <c r="F30" s="62" t="n"/>
-      <c r="G30" s="62" t="n"/>
-      <c r="H30" s="62" t="n"/>
-      <c r="I30" s="62" t="n"/>
-      <c r="J30" s="62" t="n"/>
+      <c r="F30" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="62" t="n">
+        <v>350</v>
+      </c>
       <c r="K30" s="62" t="n"/>
       <c r="L30" s="62" t="n"/>
       <c r="M30" s="62" t="n"/>
@@ -1686,19 +2082,37 @@
       <c r="T30" s="62" t="n"/>
     </row>
     <row r="31" ht="15.75" customHeight="1" s="39">
-      <c r="A31" s="58" t="n"/>
+      <c r="A31" s="58" t="inlineStr">
+        <is>
+          <t>6338555</t>
+        </is>
+      </c>
       <c r="B31" s="59" t="n"/>
       <c r="C31" s="60" t="n"/>
-      <c r="D31" s="60" t="n"/>
+      <c r="D31" s="60" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
       <c r="E31" s="61">
         <f>SUM(F31:T31)</f>
         <v/>
       </c>
-      <c r="F31" s="62" t="n"/>
-      <c r="G31" s="62" t="n"/>
-      <c r="H31" s="62" t="n"/>
-      <c r="I31" s="62" t="n"/>
-      <c r="J31" s="62" t="n"/>
+      <c r="F31" s="62" t="n">
+        <v>900</v>
+      </c>
+      <c r="G31" s="62" t="n">
+        <v>200</v>
+      </c>
+      <c r="H31" s="62" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" s="62" t="n">
+        <v>400</v>
+      </c>
+      <c r="J31" s="62" t="n">
+        <v>0</v>
+      </c>
       <c r="K31" s="62" t="n"/>
       <c r="L31" s="62" t="n"/>
       <c r="M31" s="62" t="n"/>
@@ -2734,7 +3148,7 @@
     <row r="67" ht="13.8" customHeight="1" s="39">
       <c r="A67" s="63" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1147</t>
         </is>
       </c>
       <c r="B67" s="64" t="n"/>
@@ -2751,19 +3165,19 @@
         <v/>
       </c>
       <c r="F67" s="65" t="n">
-        <v>7897987978992</v>
+        <v>305</v>
       </c>
       <c r="G67" s="65" t="n">
-        <v>8</v>
+        <v>125</v>
       </c>
       <c r="H67" s="65" t="n">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="I67" s="65" t="n">
-        <v>59</v>
+        <v>925</v>
       </c>
       <c r="J67" s="65" t="n">
-        <v>7</v>
+        <v>250</v>
       </c>
       <c r="K67" s="65" t="n"/>
       <c r="L67" s="65" t="n"/>
@@ -2777,21 +3191,39 @@
       <c r="T67" s="65" t="n"/>
     </row>
     <row r="68" ht="13.8" customHeight="1" s="39">
-      <c r="A68" s="63" t="n"/>
+      <c r="A68" s="63" t="inlineStr">
+        <is>
+          <t>364</t>
+        </is>
+      </c>
       <c r="B68" s="64" t="n"/>
       <c r="C68" s="60" t="n">
         <v>44074</v>
       </c>
-      <c r="D68" s="60" t="n"/>
+      <c r="D68" s="60" t="inlineStr">
+        <is>
+          <t>Deliver</t>
+        </is>
+      </c>
       <c r="E68" s="66">
         <f>SUM(F68:T68)</f>
         <v/>
       </c>
-      <c r="F68" s="65" t="n"/>
-      <c r="G68" s="65" t="n"/>
-      <c r="H68" s="65" t="n"/>
-      <c r="I68" s="65" t="n"/>
-      <c r="J68" s="65" t="n"/>
+      <c r="F68" s="65" t="n">
+        <v>1885</v>
+      </c>
+      <c r="G68" s="65" t="n">
+        <v>550</v>
+      </c>
+      <c r="H68" s="65" t="n">
+        <v>880</v>
+      </c>
+      <c r="I68" s="65" t="n">
+        <v>6160</v>
+      </c>
+      <c r="J68" s="65" t="n">
+        <v>100</v>
+      </c>
       <c r="K68" s="65" t="n"/>
       <c r="L68" s="65" t="n"/>
       <c r="M68" s="65" t="n"/>
@@ -2804,21 +3236,39 @@
       <c r="T68" s="65" t="n"/>
     </row>
     <row r="69" ht="13.8" customHeight="1" s="39">
-      <c r="A69" s="63" t="n"/>
+      <c r="A69" s="63" t="inlineStr">
+        <is>
+          <t>483</t>
+        </is>
+      </c>
       <c r="B69" s="64" t="n"/>
       <c r="C69" s="60" t="n">
         <v>44074</v>
       </c>
-      <c r="D69" s="60" t="n"/>
+      <c r="D69" s="60" t="inlineStr">
+        <is>
+          <t>Deliver</t>
+        </is>
+      </c>
       <c r="E69" s="66">
         <f>SUM(F69:T69)</f>
         <v/>
       </c>
-      <c r="F69" s="65" t="n"/>
-      <c r="G69" s="65" t="n"/>
-      <c r="H69" s="65" t="n"/>
-      <c r="I69" s="65" t="n"/>
-      <c r="J69" s="65" t="n"/>
+      <c r="F69" s="65" t="n">
+        <v>3060</v>
+      </c>
+      <c r="G69" s="65" t="n">
+        <v>875</v>
+      </c>
+      <c r="H69" s="65" t="n">
+        <v>95</v>
+      </c>
+      <c r="I69" s="65" t="n">
+        <v>3985</v>
+      </c>
+      <c r="J69" s="65" t="n">
+        <v>855</v>
+      </c>
       <c r="K69" s="65" t="n"/>
       <c r="L69" s="65" t="n"/>
       <c r="M69" s="65" t="n"/>
@@ -2831,21 +3281,39 @@
       <c r="T69" s="65" t="n"/>
     </row>
     <row r="70" ht="13.8" customHeight="1" s="39">
-      <c r="A70" s="63" t="n"/>
+      <c r="A70" s="63" t="inlineStr">
+        <is>
+          <t>1255</t>
+        </is>
+      </c>
       <c r="B70" s="64" t="n"/>
       <c r="C70" s="60" t="n">
         <v>44074</v>
       </c>
-      <c r="D70" s="60" t="n"/>
+      <c r="D70" s="60" t="inlineStr">
+        <is>
+          <t>Deliver</t>
+        </is>
+      </c>
       <c r="E70" s="66">
         <f>SUM(F70:T70)</f>
         <v/>
       </c>
-      <c r="F70" s="65" t="n"/>
-      <c r="G70" s="65" t="n"/>
-      <c r="H70" s="65" t="n"/>
-      <c r="I70" s="65" t="n"/>
-      <c r="J70" s="65" t="n"/>
+      <c r="F70" s="65" t="n">
+        <v>2875</v>
+      </c>
+      <c r="G70" s="65" t="n">
+        <v>625</v>
+      </c>
+      <c r="H70" s="65" t="n">
+        <v>0</v>
+      </c>
+      <c r="I70" s="65" t="n">
+        <v>1200</v>
+      </c>
+      <c r="J70" s="65" t="n">
+        <v>760</v>
+      </c>
       <c r="K70" s="65" t="n"/>
       <c r="L70" s="65" t="n"/>
       <c r="M70" s="65" t="n"/>

</xml_diff>